<commit_message>
April Access Logs Updated(15 to 27)
</commit_message>
<xml_diff>
--- a/Attendance(SulajAcharya)/March_Attendance(SulajAcharya).xlsx
+++ b/Attendance(SulajAcharya)/March_Attendance(SulajAcharya).xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sulaj Acharya\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SulajAcharya\Godrej\Attendance(SulajAcharya)\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B76ADA8-6ABE-4AD0-8FD8-C70775891E09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3333383-5A36-4F9B-8A91-D40BEC574367}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,9 +26,6 @@
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="8">
-  <si>
-    <t>TEAM ATTENDANCE - FEBRUARY 2025</t>
-  </si>
   <si>
     <t>NAME</t>
   </si>
@@ -49,6 +46,9 @@
   </si>
   <si>
     <t>Holiday For Holi</t>
+  </si>
+  <si>
+    <t>TEAM ATTENDANCE - MARCH 2025</t>
   </si>
 </sst>
 </file>
@@ -552,16 +552,7 @@
     <xf numFmtId="0" fontId="7" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="10" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -573,13 +564,22 @@
     <xf numFmtId="14" fontId="1" fillId="6" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -588,16 +588,16 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -818,7 +818,7 @@
   <dimension ref="A1:X989"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1"/>
@@ -834,8 +834,8 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="14.4">
-      <c r="A1" s="50" t="s">
-        <v>0</v>
+      <c r="A1" s="59" t="s">
+        <v>7</v>
       </c>
       <c r="B1" s="60"/>
       <c r="C1" s="61"/>
@@ -862,11 +862,11 @@
       <c r="X1" s="4"/>
     </row>
     <row r="2" spans="1:24" ht="14.4">
-      <c r="A2" s="51" t="s">
-        <v>1</v>
+      <c r="A2" s="62" t="s">
+        <v>0</v>
       </c>
-      <c r="B2" s="62"/>
-      <c r="C2" s="63"/>
+      <c r="B2" s="63"/>
+      <c r="C2" s="64"/>
       <c r="D2" s="5"/>
       <c r="E2" s="6"/>
       <c r="F2" s="6"/>
@@ -890,13 +890,13 @@
       <c r="X2" s="4"/>
     </row>
     <row r="3" spans="1:24" ht="14.4">
-      <c r="A3" s="52" t="s">
+      <c r="A3" s="50" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="65" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="53" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" s="63"/>
+      <c r="C3" s="64"/>
       <c r="D3" s="10"/>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
@@ -920,22 +920,22 @@
       <c r="X3" s="4"/>
     </row>
     <row r="4" spans="1:24" ht="14.4">
-      <c r="A4" s="54">
+      <c r="A4" s="51">
         <v>45717</v>
       </c>
-      <c r="B4" s="55" t="s">
-        <v>4</v>
+      <c r="B4" s="52" t="s">
+        <v>3</v>
       </c>
-      <c r="C4" s="64"/>
+      <c r="C4" s="56"/>
     </row>
     <row r="5" spans="1:24" thickBot="1">
-      <c r="A5" s="56">
+      <c r="A5" s="53">
         <v>45718</v>
       </c>
       <c r="B5" s="57" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
-      <c r="C5" s="65"/>
+      <c r="C5" s="58"/>
       <c r="D5" s="16"/>
       <c r="E5" s="11"/>
       <c r="F5" s="11"/>
@@ -959,13 +959,13 @@
       <c r="X5" s="4"/>
     </row>
     <row r="6" spans="1:24" thickBot="1">
-      <c r="A6" s="54">
+      <c r="A6" s="51">
         <v>45719</v>
       </c>
-      <c r="B6" s="55" t="s">
-        <v>4</v>
+      <c r="B6" s="52" t="s">
+        <v>3</v>
       </c>
-      <c r="C6" s="55"/>
+      <c r="C6" s="52"/>
       <c r="D6" s="17"/>
       <c r="E6" s="18"/>
       <c r="F6" s="19"/>
@@ -989,13 +989,13 @@
       <c r="X6" s="4"/>
     </row>
     <row r="7" spans="1:24" thickBot="1">
-      <c r="A7" s="54">
+      <c r="A7" s="51">
         <v>45720</v>
       </c>
-      <c r="B7" s="55" t="s">
-        <v>4</v>
+      <c r="B7" s="52" t="s">
+        <v>3</v>
       </c>
-      <c r="C7" s="55"/>
+      <c r="C7" s="52"/>
       <c r="D7" s="22"/>
       <c r="E7" s="23"/>
       <c r="F7" s="24"/>
@@ -1019,13 +1019,13 @@
       <c r="X7" s="4"/>
     </row>
     <row r="8" spans="1:24" thickBot="1">
-      <c r="A8" s="54">
+      <c r="A8" s="51">
         <v>45721</v>
       </c>
-      <c r="B8" s="55" t="s">
-        <v>4</v>
+      <c r="B8" s="52" t="s">
+        <v>3</v>
       </c>
-      <c r="C8" s="55"/>
+      <c r="C8" s="52"/>
       <c r="D8" s="25"/>
       <c r="E8" s="23"/>
       <c r="F8" s="17"/>
@@ -1049,13 +1049,13 @@
       <c r="X8" s="4"/>
     </row>
     <row r="9" spans="1:24" thickBot="1">
-      <c r="A9" s="54">
+      <c r="A9" s="51">
         <v>45722</v>
       </c>
-      <c r="B9" s="55" t="s">
-        <v>4</v>
+      <c r="B9" s="52" t="s">
+        <v>3</v>
       </c>
-      <c r="C9" s="58"/>
+      <c r="C9" s="54"/>
       <c r="D9" s="22"/>
       <c r="E9" s="23"/>
       <c r="F9" s="24"/>
@@ -1079,13 +1079,13 @@
       <c r="X9" s="4"/>
     </row>
     <row r="10" spans="1:24" thickBot="1">
-      <c r="A10" s="54">
+      <c r="A10" s="51">
         <v>45723</v>
       </c>
-      <c r="B10" s="55" t="s">
-        <v>4</v>
+      <c r="B10" s="52" t="s">
+        <v>3</v>
       </c>
-      <c r="C10" s="58"/>
+      <c r="C10" s="54"/>
       <c r="D10" s="22"/>
       <c r="E10" s="23"/>
       <c r="F10" s="24"/>
@@ -1109,13 +1109,13 @@
       <c r="X10" s="4"/>
     </row>
     <row r="11" spans="1:24" thickBot="1">
-      <c r="A11" s="54">
+      <c r="A11" s="51">
         <v>45724</v>
       </c>
-      <c r="B11" s="55" t="s">
-        <v>4</v>
+      <c r="B11" s="52" t="s">
+        <v>3</v>
       </c>
-      <c r="C11" s="58"/>
+      <c r="C11" s="54"/>
       <c r="D11" s="22"/>
       <c r="E11" s="23"/>
       <c r="F11" s="24"/>
@@ -1139,13 +1139,13 @@
       <c r="X11" s="4"/>
     </row>
     <row r="12" spans="1:24" thickBot="1">
-      <c r="A12" s="56">
+      <c r="A12" s="53">
         <v>45725</v>
       </c>
       <c r="B12" s="57" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
-      <c r="C12" s="65"/>
+      <c r="C12" s="58"/>
       <c r="D12" s="26"/>
       <c r="E12" s="23"/>
       <c r="F12" s="27"/>
@@ -1169,13 +1169,13 @@
       <c r="X12" s="4"/>
     </row>
     <row r="13" spans="1:24" thickBot="1">
-      <c r="A13" s="54">
+      <c r="A13" s="51">
         <v>45726</v>
       </c>
-      <c r="B13" s="55" t="s">
-        <v>4</v>
+      <c r="B13" s="52" t="s">
+        <v>3</v>
       </c>
-      <c r="C13" s="55"/>
+      <c r="C13" s="52"/>
       <c r="D13" s="24"/>
       <c r="E13" s="30"/>
       <c r="F13" s="11"/>
@@ -1199,13 +1199,13 @@
       <c r="X13" s="4"/>
     </row>
     <row r="14" spans="1:24" thickBot="1">
-      <c r="A14" s="54">
+      <c r="A14" s="51">
         <v>45727</v>
       </c>
-      <c r="B14" s="55" t="s">
-        <v>4</v>
+      <c r="B14" s="52" t="s">
+        <v>3</v>
       </c>
-      <c r="C14" s="55"/>
+      <c r="C14" s="52"/>
       <c r="D14" s="31"/>
       <c r="E14" s="4"/>
       <c r="F14" s="4"/>
@@ -1229,13 +1229,13 @@
       <c r="X14" s="4"/>
     </row>
     <row r="15" spans="1:24" thickBot="1">
-      <c r="A15" s="54">
+      <c r="A15" s="51">
         <v>45728</v>
       </c>
-      <c r="B15" s="55" t="s">
-        <v>4</v>
+      <c r="B15" s="52" t="s">
+        <v>3</v>
       </c>
-      <c r="C15" s="55"/>
+      <c r="C15" s="52"/>
       <c r="D15" s="32"/>
       <c r="E15" s="4"/>
       <c r="F15" s="4"/>
@@ -1259,13 +1259,13 @@
       <c r="X15" s="4"/>
     </row>
     <row r="16" spans="1:24" thickBot="1">
-      <c r="A16" s="54">
+      <c r="A16" s="51">
         <v>45729</v>
       </c>
-      <c r="B16" s="55" t="s">
-        <v>4</v>
+      <c r="B16" s="52" t="s">
+        <v>3</v>
       </c>
-      <c r="C16" s="58"/>
+      <c r="C16" s="54"/>
       <c r="D16" s="33"/>
       <c r="E16" s="31"/>
       <c r="F16" s="4"/>
@@ -1289,14 +1289,14 @@
       <c r="X16" s="4"/>
     </row>
     <row r="17" spans="1:24" thickBot="1">
-      <c r="A17" s="54">
+      <c r="A17" s="51">
         <v>45730</v>
       </c>
-      <c r="B17" s="55" t="s">
+      <c r="B17" s="52" t="s">
+        <v>5</v>
+      </c>
+      <c r="C17" s="55" t="s">
         <v>6</v>
-      </c>
-      <c r="C17" s="59" t="s">
-        <v>7</v>
       </c>
       <c r="D17" s="34"/>
       <c r="E17" s="31"/>
@@ -1321,13 +1321,13 @@
       <c r="X17" s="4"/>
     </row>
     <row r="18" spans="1:24" thickBot="1">
-      <c r="A18" s="54">
+      <c r="A18" s="51">
         <v>45731</v>
       </c>
-      <c r="B18" s="55" t="s">
-        <v>4</v>
+      <c r="B18" s="52" t="s">
+        <v>3</v>
       </c>
-      <c r="C18" s="58"/>
+      <c r="C18" s="54"/>
       <c r="D18" s="33"/>
       <c r="E18" s="31"/>
       <c r="F18" s="4"/>
@@ -1351,13 +1351,13 @@
       <c r="X18" s="4"/>
     </row>
     <row r="19" spans="1:24" thickBot="1">
-      <c r="A19" s="56">
+      <c r="A19" s="53">
         <v>45732</v>
       </c>
       <c r="B19" s="57" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
-      <c r="C19" s="65"/>
+      <c r="C19" s="58"/>
       <c r="D19" s="34"/>
       <c r="E19" s="31"/>
       <c r="F19" s="4"/>
@@ -1381,13 +1381,13 @@
       <c r="X19" s="4"/>
     </row>
     <row r="20" spans="1:24" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A20" s="54">
+      <c r="A20" s="51">
         <v>45733</v>
       </c>
-      <c r="B20" s="55" t="s">
-        <v>4</v>
+      <c r="B20" s="52" t="s">
+        <v>3</v>
       </c>
-      <c r="C20" s="55"/>
+      <c r="C20" s="52"/>
       <c r="D20" s="33"/>
       <c r="E20" s="31"/>
       <c r="F20" s="4"/>
@@ -1411,13 +1411,13 @@
       <c r="X20" s="4"/>
     </row>
     <row r="21" spans="1:24" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A21" s="54">
+      <c r="A21" s="51">
         <v>45734</v>
       </c>
-      <c r="B21" s="55" t="s">
-        <v>4</v>
+      <c r="B21" s="52" t="s">
+        <v>3</v>
       </c>
-      <c r="C21" s="55"/>
+      <c r="C21" s="52"/>
       <c r="D21" s="33"/>
       <c r="E21" s="31"/>
       <c r="F21" s="4"/>
@@ -1441,13 +1441,13 @@
       <c r="X21" s="4"/>
     </row>
     <row r="22" spans="1:24" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A22" s="54">
+      <c r="A22" s="51">
         <v>45735</v>
       </c>
-      <c r="B22" s="55" t="s">
-        <v>4</v>
+      <c r="B22" s="52" t="s">
+        <v>3</v>
       </c>
-      <c r="C22" s="55"/>
+      <c r="C22" s="52"/>
       <c r="D22" s="33"/>
       <c r="E22" s="31"/>
       <c r="F22" s="4"/>
@@ -1471,13 +1471,13 @@
       <c r="X22" s="4"/>
     </row>
     <row r="23" spans="1:24" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A23" s="54">
+      <c r="A23" s="51">
         <v>45736</v>
       </c>
-      <c r="B23" s="55" t="s">
-        <v>4</v>
+      <c r="B23" s="52" t="s">
+        <v>3</v>
       </c>
-      <c r="C23" s="58"/>
+      <c r="C23" s="54"/>
       <c r="D23" s="33"/>
       <c r="E23" s="31"/>
       <c r="F23" s="4"/>
@@ -1501,13 +1501,13 @@
       <c r="X23" s="4"/>
     </row>
     <row r="24" spans="1:24" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A24" s="54">
+      <c r="A24" s="51">
         <v>45737</v>
       </c>
-      <c r="B24" s="55" t="s">
-        <v>4</v>
+      <c r="B24" s="52" t="s">
+        <v>3</v>
       </c>
-      <c r="C24" s="58"/>
+      <c r="C24" s="54"/>
       <c r="D24" s="35"/>
       <c r="E24" s="31"/>
       <c r="F24" s="8"/>
@@ -1531,13 +1531,13 @@
       <c r="X24" s="4"/>
     </row>
     <row r="25" spans="1:24" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A25" s="54">
+      <c r="A25" s="51">
         <v>45738</v>
       </c>
-      <c r="B25" s="55" t="s">
-        <v>4</v>
+      <c r="B25" s="52" t="s">
+        <v>3</v>
       </c>
-      <c r="C25" s="58"/>
+      <c r="C25" s="54"/>
       <c r="D25" s="37"/>
       <c r="E25" s="31"/>
       <c r="F25" s="38"/>
@@ -1561,13 +1561,13 @@
       <c r="X25" s="4"/>
     </row>
     <row r="26" spans="1:24" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A26" s="56">
+      <c r="A26" s="53">
         <v>45739</v>
       </c>
       <c r="B26" s="57" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
-      <c r="C26" s="65"/>
+      <c r="C26" s="58"/>
       <c r="D26" s="40"/>
       <c r="E26" s="31"/>
       <c r="F26" s="8"/>
@@ -1591,13 +1591,13 @@
       <c r="X26" s="4"/>
     </row>
     <row r="27" spans="1:24" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A27" s="54">
+      <c r="A27" s="51">
         <v>45740</v>
       </c>
-      <c r="B27" s="55" t="s">
-        <v>4</v>
+      <c r="B27" s="52" t="s">
+        <v>3</v>
       </c>
-      <c r="C27" s="55"/>
+      <c r="C27" s="52"/>
       <c r="D27" s="37"/>
       <c r="E27" s="31"/>
       <c r="F27" s="38"/>
@@ -1621,13 +1621,13 @@
       <c r="X27" s="4"/>
     </row>
     <row r="28" spans="1:24" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A28" s="54">
+      <c r="A28" s="51">
         <v>45741</v>
       </c>
-      <c r="B28" s="55" t="s">
-        <v>4</v>
+      <c r="B28" s="52" t="s">
+        <v>3</v>
       </c>
-      <c r="C28" s="55"/>
+      <c r="C28" s="52"/>
       <c r="D28" s="35"/>
       <c r="E28" s="31"/>
       <c r="F28" s="8"/>
@@ -1651,13 +1651,13 @@
       <c r="X28" s="4"/>
     </row>
     <row r="29" spans="1:24" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A29" s="54">
+      <c r="A29" s="51">
         <v>45742</v>
       </c>
-      <c r="B29" s="55" t="s">
-        <v>4</v>
+      <c r="B29" s="52" t="s">
+        <v>3</v>
       </c>
-      <c r="C29" s="55"/>
+      <c r="C29" s="52"/>
       <c r="D29" s="37"/>
       <c r="E29" s="31"/>
       <c r="F29" s="38"/>
@@ -1681,13 +1681,13 @@
       <c r="X29" s="4"/>
     </row>
     <row r="30" spans="1:24" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A30" s="54">
+      <c r="A30" s="51">
         <v>45743</v>
       </c>
-      <c r="B30" s="55" t="s">
-        <v>4</v>
+      <c r="B30" s="52" t="s">
+        <v>3</v>
       </c>
-      <c r="C30" s="58"/>
+      <c r="C30" s="54"/>
       <c r="D30" s="35"/>
       <c r="E30" s="31"/>
       <c r="F30" s="8"/>
@@ -1711,13 +1711,13 @@
       <c r="X30" s="4"/>
     </row>
     <row r="31" spans="1:24" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A31" s="54">
+      <c r="A31" s="51">
         <v>45744</v>
       </c>
-      <c r="B31" s="55" t="s">
-        <v>4</v>
+      <c r="B31" s="52" t="s">
+        <v>3</v>
       </c>
-      <c r="C31" s="58"/>
+      <c r="C31" s="54"/>
       <c r="D31" s="37"/>
       <c r="E31" s="31"/>
       <c r="F31" s="38"/>
@@ -1741,13 +1741,13 @@
       <c r="X31" s="4"/>
     </row>
     <row r="32" spans="1:24" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A32" s="54">
+      <c r="A32" s="51">
         <v>45745</v>
       </c>
-      <c r="B32" s="55" t="s">
-        <v>4</v>
+      <c r="B32" s="52" t="s">
+        <v>3</v>
       </c>
-      <c r="C32" s="58"/>
+      <c r="C32" s="54"/>
       <c r="D32" s="37"/>
       <c r="E32" s="31"/>
       <c r="F32" s="38"/>
@@ -1771,13 +1771,13 @@
       <c r="X32" s="4"/>
     </row>
     <row r="33" spans="1:24" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A33" s="56">
+      <c r="A33" s="53">
         <v>45746</v>
       </c>
       <c r="B33" s="57" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
-      <c r="C33" s="65"/>
+      <c r="C33" s="58"/>
       <c r="D33" s="35"/>
       <c r="E33" s="31"/>
       <c r="F33" s="8"/>
@@ -1801,13 +1801,13 @@
       <c r="X33" s="4"/>
     </row>
     <row r="34" spans="1:24" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A34" s="54">
+      <c r="A34" s="51">
         <v>45747</v>
       </c>
-      <c r="B34" s="55" t="s">
-        <v>4</v>
+      <c r="B34" s="52" t="s">
+        <v>3</v>
       </c>
-      <c r="C34" s="58"/>
+      <c r="C34" s="54"/>
       <c r="D34" s="37"/>
       <c r="E34" s="31"/>
       <c r="F34" s="38"/>

</xml_diff>